<commit_message>
Hoàn thiện nhận xét cơ bản về đại vận
</commit_message>
<xml_diff>
--- a/Luandaivan.xlsx
+++ b/Luandaivan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14D3664-944E-4889-B03D-C97FC28929FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92D098B-1B9F-4671-9883-674848B5A120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,19 +42,19 @@
     <t>Tam hợp đại vận đồng hành với Tam hợp tuổi</t>
   </si>
   <si>
-    <t>Đại vận rất xấu, sẽ gặp nhiều khó khăn và buồn lo.</t>
-  </si>
-  <si>
-    <t>Đại đẹp sẽ gặp nhiều việc toại ý.</t>
-  </si>
-  <si>
-    <t>Đại vận đại cát sẽ gặp nhiều việc tốt, nhiều cơ hội, thuận với bản thân.</t>
-  </si>
-  <si>
     <t>Đại vận sinh xuất gặp nhiều lao đao, nhưng có nghị lực vẫn gặt quả ngọt.</t>
   </si>
   <si>
-    <t>Đại vận xấu, sẽ phải cố gắng làm nhưng để trả nợ đời.</t>
+    <t>Đại vận đẹp sẽ gặp nhiều việc toại ý.</t>
+  </si>
+  <si>
+    <t>Đại vận xấu, sẽ phải cố gắng lắm nhưng cũng để trả nợ đời. Âu cũng phải cố gắng vì làm gì có nợ nào mà không phải trả.</t>
+  </si>
+  <si>
+    <t>Đại vận đại cát sẽ gặp nhiều việc tốt, nhiều cơ hội, thuận lợi với bản thân.</t>
+  </si>
+  <si>
+    <t>Đại vận rất xấu, sẽ gặp nhiều khó khăn và buồn lo. Nhưng sẽ có nhiều bài học sâu sắc.</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +389,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -397,7 +397,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -413,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hoàn thiện luận cung đại vận
</commit_message>
<xml_diff>
--- a/Luandaivan.xlsx
+++ b/Luandaivan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92D098B-1B9F-4671-9883-674848B5A120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7452FBB5-E077-4E3A-9B69-63EB444EFB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Tam hợp tuổi sinh Tam hợp đại vận</t>
   </si>
@@ -55,6 +55,36 @@
   </si>
   <si>
     <t>Đại vận rất xấu, sẽ gặp nhiều khó khăn và buồn lo. Nhưng sẽ có nhiều bài học sâu sắc.</t>
+  </si>
+  <si>
+    <t>Ngũ hành bản Mệnh sinh Ngũ hành cung đại vận</t>
+  </si>
+  <si>
+    <t>Ngũ hành bản Mệnh khắc Ngũ hành cung đại vận</t>
+  </si>
+  <si>
+    <t>Ngũ hành cung đại vận sinh Ngũ hành bản Mệnh</t>
+  </si>
+  <si>
+    <t>Ngũ hành cung đại vận khắc Ngũ hành bản Mệnh</t>
+  </si>
+  <si>
+    <t>Ngũ hành cung đại vận đồng hành với Ngũ hành bản Mệnh</t>
+  </si>
+  <si>
+    <t>Bản thân tổn hao sức khỏe, tiền bạc, công sức. Phải dụng công sức trí lực để hưởng trái ngọt.</t>
+  </si>
+  <si>
+    <t>Cuộc sống thuận lợi, có nhiều cơ hội cho bản thân phát triển.</t>
+  </si>
+  <si>
+    <t>Cuộc bế tắc, bản thân gặp trì trệ, không có nhiều bứt phá.</t>
+  </si>
+  <si>
+    <t>Cuộc sống có nhiều thuận lợi, bản thân có nhiều cơ hội và may mắn bất ngờ.</t>
+  </si>
+  <si>
+    <t>Cuộc sống gặp nhiều khó khăn, bản thân phải năng động để có cuộc sống tốt hơn.</t>
   </si>
 </sst>
 </file>
@@ -372,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -424,6 +454,46 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>